<commit_message>
Add bio master E
</commit_message>
<xml_diff>
--- a/src/Prototypes/hmi/AI/bio_master_A.xlsx
+++ b/src/Prototypes/hmi/AI/bio_master_A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q\Documents\uni\Echo-HMI\AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q\Documents\uni\Echo\Project-Echo\src\Prototypes\hmi\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88BB96E-5E57-497A-B491-F25872914183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CF9B06-2522-4B09-8771-72F03F392E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="5700" windowWidth="24300" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="4100" windowWidth="25520" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bio_master_D" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="195">
   <si>
     <t>Animal</t>
   </si>
@@ -246,72 +246,6 @@
     <t>Ceyx azureus</t>
   </si>
   <si>
-    <t>Chalcites basalis</t>
-  </si>
-  <si>
-    <t>Chalcites lucidus</t>
-  </si>
-  <si>
-    <t>Chalcites osculans</t>
-  </si>
-  <si>
-    <t>Chelapsalta puer</t>
-  </si>
-  <si>
-    <t>Chenonetta jubata</t>
-  </si>
-  <si>
-    <t>Cherax destructor</t>
-  </si>
-  <si>
-    <t>Chlamydera guttata</t>
-  </si>
-  <si>
-    <t>Chlamydera nuchalis</t>
-  </si>
-  <si>
-    <t>CicadidaeÂ sp.</t>
-  </si>
-  <si>
-    <t>Cincloramphus mathewsi</t>
-  </si>
-  <si>
-    <t>Cinclosoma cinnamomeum</t>
-  </si>
-  <si>
-    <t>Cinclosoma punctatum</t>
-  </si>
-  <si>
-    <t>Cisticola exilis</t>
-  </si>
-  <si>
-    <t>Climacteris erythrops</t>
-  </si>
-  <si>
-    <t>Climacteris picumnus</t>
-  </si>
-  <si>
-    <t>Colluricincla harmonica</t>
-  </si>
-  <si>
-    <t>Colluricincla megarhyncha</t>
-  </si>
-  <si>
-    <t>Colluricincla woodwardi</t>
-  </si>
-  <si>
-    <t>Conocephalus albescens</t>
-  </si>
-  <si>
-    <t>Conocephalus semivittatus</t>
-  </si>
-  <si>
-    <t>Conocephalus upoluensis</t>
-  </si>
-  <si>
-    <t>ConocephalusÂ sp.</t>
-  </si>
-  <si>
     <t>Bio Prompt</t>
   </si>
   <si>
@@ -507,72 +441,6 @@
     <t>A photo realistic images of the animal, Ceyx azureus in it's natural habitat</t>
   </si>
   <si>
-    <t>A photo realistic images of the animal, Chalcites basalis in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chalcites lucidus in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chalcites osculans in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chelapsalta puer in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chenonetta jubata in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Cherax destructor in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chlamydera guttata in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Chlamydera nuchalis in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, CicadidaeÂ sp. in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Cincloramphus mathewsi in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Cinclosoma cinnamomeum in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Cinclosoma punctatum in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Cisticola exilis in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Climacteris erythrops in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Climacteris picumnus in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Colluricincla harmonica in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Colluricincla megarhyncha in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Colluricincla woodwardi in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Conocephalus albescens in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Conocephalus semivittatus in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, Conocephalus upoluensis in it's natural habitat</t>
-  </si>
-  <si>
-    <t>A photo realistic images of the animal, ConocephalusÂ sp. in it's natural habitat</t>
-  </si>
-  <si>
     <t>Please generate a short species bio with some interesting facts about  Acanthagenys rufogularis.</t>
   </si>
   <si>
@@ -754,72 +622,6 @@
   </si>
   <si>
     <t>Please generate a short species bio with some interesting facts about  Ceyx azureus.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chalcites basalis.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chalcites lucidus.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chalcites osculans.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chelapsalta puer.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chenonetta jubata.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Cherax destructor.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chlamydera guttata.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Chlamydera nuchalis.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  CicadidaeÂ sp..</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Cincloramphus mathewsi.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Cinclosoma cinnamomeum.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Cinclosoma punctatum.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Cisticola exilis.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Climacteris erythrops.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Climacteris picumnus.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Colluricincla harmonica.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Colluricincla megarhyncha.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Colluricincla woodwardi.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Conocephalus albescens.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Conocephalus semivittatus.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  Conocephalus upoluensis.</t>
-  </si>
-  <si>
-    <t>Please generate a short species bio with some interesting facts about  ConocephalusÂ sp..</t>
   </si>
   <si>
     <t>Common Name</t>
@@ -1994,11 +1796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A62:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2026,13 +1828,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>260</v>
+        <v>194</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
@@ -2060,10 +1862,10 @@
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="12" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="22"/>
@@ -2076,20 +1878,20 @@
         <v>A photo realistic images of the animal, Acanthagenys rufogularis in it's natural habitat</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="O2" t="str">
         <f>_xlfn.CONCAT($P$2,A2,$Q$2)</f>
         <v>Please generate a short species bio with some interesting facts about  Acanthagenys rufogularis.</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
-        <v>178</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2097,17 +1899,17 @@
         <v>8</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="L3" s="9" t="str">
-        <f t="shared" ref="L3:L66" si="0">_xlfn.CONCAT($M$2,A3,$N$2)</f>
+        <f t="shared" ref="L3:L61" si="0">_xlfn.CONCAT($M$2,A3,$N$2)</f>
         <v>A photo realistic images of the animal, Acanthiza apicalis in it's natural habitat</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O66" si="1">_xlfn.CONCAT($P$2,A3,$Q$2)</f>
+        <f t="shared" ref="O3:O61" si="1">_xlfn.CONCAT($P$2,A3,$Q$2)</f>
         <v>Please generate a short species bio with some interesting facts about  Acanthiza apicalis.</v>
       </c>
     </row>
@@ -2116,10 +1918,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="L4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2136,10 +1938,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="L5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2155,10 +1957,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="L6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2174,10 +1976,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="L7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2193,10 +1995,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="L8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2212,10 +2014,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="L9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2231,10 +2033,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="L10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2250,10 +2052,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="L11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2269,10 +2071,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="L12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2288,10 +2090,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="L13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2307,10 +2109,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="L14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2326,10 +2128,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>21</v>
@@ -2348,10 +2150,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="L16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2367,10 +2169,10 @@
         <v>23</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="L17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2386,10 +2188,10 @@
         <v>24</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>21</v>
@@ -2408,10 +2210,10 @@
         <v>25</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="L19" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2427,10 +2229,10 @@
         <v>26</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="L20" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2446,10 +2248,10 @@
         <v>27</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2465,10 +2267,10 @@
         <v>28</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="L22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2484,10 +2286,10 @@
         <v>29</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="L23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2503,10 +2305,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="L24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2522,10 +2324,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="L25" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2541,10 +2343,10 @@
         <v>32</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="L26" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2560,10 +2362,10 @@
         <v>33</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="L27" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2579,10 +2381,10 @@
         <v>34</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="L28" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2598,10 +2400,10 @@
         <v>35</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="L29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2617,10 +2419,10 @@
         <v>36</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>206</v>
+        <v>162</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="L30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2636,10 +2438,10 @@
         <v>37</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="L31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2655,10 +2457,10 @@
         <v>38</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>208</v>
+        <v>164</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="L32" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2674,10 +2476,10 @@
         <v>39</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="L33" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2693,10 +2495,10 @@
         <v>40</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="L34" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2712,10 +2514,10 @@
         <v>41</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="L35" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2731,10 +2533,10 @@
         <v>42</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="L36" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2750,10 +2552,10 @@
         <v>43</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="L37" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2769,10 +2571,10 @@
         <v>44</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="L38" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2788,10 +2590,10 @@
         <v>45</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="L39" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2807,10 +2609,10 @@
         <v>46</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="L40" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2826,10 +2628,10 @@
         <v>47</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="L41" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2845,10 +2647,10 @@
         <v>48</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="L42" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2864,10 +2666,10 @@
         <v>49</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="L43" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2883,10 +2685,10 @@
         <v>50</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="L44" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2902,10 +2704,10 @@
         <v>51</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="L45" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2921,10 +2723,10 @@
         <v>52</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="L46" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2940,10 +2742,10 @@
         <v>53</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="L47" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2959,10 +2761,10 @@
         <v>54</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>224</v>
+        <v>180</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="L48" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2978,10 +2780,10 @@
         <v>55</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="L49" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2997,10 +2799,10 @@
         <v>56</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="L50" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3016,10 +2818,10 @@
         <v>57</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="F51" s="28" t="s">
         <v>21</v>
@@ -3038,10 +2840,10 @@
         <v>58</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="L52" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3057,10 +2859,10 @@
         <v>59</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="L53" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3076,10 +2878,10 @@
         <v>60</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="L54" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3095,10 +2897,10 @@
         <v>61</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="L55" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3114,10 +2916,10 @@
         <v>62</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="F56" s="28" t="s">
         <v>21</v>
@@ -3136,10 +2938,10 @@
         <v>63</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="L57" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3155,10 +2957,10 @@
         <v>64</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="L58" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3174,10 +2976,10 @@
         <v>65</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="L59" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3193,10 +2995,10 @@
         <v>66</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="F60" s="28" t="s">
         <v>21</v>
@@ -3215,10 +3017,10 @@
         <v>67</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="L61" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3227,427 +3029,6 @@
       <c r="O61" t="str">
         <f t="shared" si="1"/>
         <v>Please generate a short species bio with some interesting facts about  Ceyx azureus.</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="L62" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Chalcites basalis in it's natural habitat</v>
-      </c>
-      <c r="O62" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Chalcites basalis.</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="L63" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Chalcites lucidus in it's natural habitat</v>
-      </c>
-      <c r="O63" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Chalcites lucidus.</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="L64" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Chalcites osculans in it's natural habitat</v>
-      </c>
-      <c r="O64" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Chalcites osculans.</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="L65" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Chelapsalta puer in it's natural habitat</v>
-      </c>
-      <c r="O65" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Chelapsalta puer.</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="L66" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Chenonetta jubata in it's natural habitat</v>
-      </c>
-      <c r="O66" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Chenonetta jubata.</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="L67" s="9" t="str">
-        <f t="shared" ref="L67:L83" si="2">_xlfn.CONCAT($M$2,A67,$N$2)</f>
-        <v>A photo realistic images of the animal, Cherax destructor in it's natural habitat</v>
-      </c>
-      <c r="O67" t="str">
-        <f t="shared" ref="O67:O83" si="3">_xlfn.CONCAT($P$2,A67,$Q$2)</f>
-        <v>Please generate a short species bio with some interesting facts about  Cherax destructor.</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="L68" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Chlamydera guttata in it's natural habitat</v>
-      </c>
-      <c r="O68" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Chlamydera guttata.</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L69" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Chlamydera nuchalis in it's natural habitat</v>
-      </c>
-      <c r="O69" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Chlamydera nuchalis.</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="L70" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, CicadidaeÂ sp. in it's natural habitat</v>
-      </c>
-      <c r="O70" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  CicadidaeÂ sp..</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="L71" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Cincloramphus mathewsi in it's natural habitat</v>
-      </c>
-      <c r="O71" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Cincloramphus mathewsi.</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="L72" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Cinclosoma cinnamomeum in it's natural habitat</v>
-      </c>
-      <c r="O72" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Cinclosoma cinnamomeum.</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="L73" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Cinclosoma punctatum in it's natural habitat</v>
-      </c>
-      <c r="O73" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Cinclosoma punctatum.</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="L74" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Cisticola exilis in it's natural habitat</v>
-      </c>
-      <c r="O74" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Cisticola exilis.</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="L75" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Climacteris erythrops in it's natural habitat</v>
-      </c>
-      <c r="O75" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Climacteris erythrops.</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L76" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Climacteris picumnus in it's natural habitat</v>
-      </c>
-      <c r="O76" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Climacteris picumnus.</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F77" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L77" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Colluricincla harmonica in it's natural habitat</v>
-      </c>
-      <c r="O77" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Colluricincla harmonica.</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="L78" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Colluricincla megarhyncha in it's natural habitat</v>
-      </c>
-      <c r="O78" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Colluricincla megarhyncha.</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="L79" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Colluricincla woodwardi in it's natural habitat</v>
-      </c>
-      <c r="O79" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Colluricincla woodwardi.</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="L80" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Conocephalus albescens in it's natural habitat</v>
-      </c>
-      <c r="O80" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Conocephalus albescens.</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="L81" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Conocephalus semivittatus in it's natural habitat</v>
-      </c>
-      <c r="O81" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Conocephalus semivittatus.</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="L82" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, Conocephalus upoluensis in it's natural habitat</v>
-      </c>
-      <c r="O82" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  Conocephalus upoluensis.</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="L83" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>A photo realistic images of the animal, ConocephalusÂ sp. in it's natural habitat</v>
-      </c>
-      <c r="O83" t="str">
-        <f t="shared" si="3"/>
-        <v>Please generate a short species bio with some interesting facts about  ConocephalusÂ sp..</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates on bio data section A
</commit_message>
<xml_diff>
--- a/src/Prototypes/hmi/AI/bio_master_A.xlsx
+++ b/src/Prototypes/hmi/AI/bio_master_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q\Documents\uni\Echo\Project-Echo\src\Prototypes\hmi\AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viett\Desktop\Deakin 2023\T1\Project-Echo\src\Prototypes\hmi\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CF9B06-2522-4B09-8771-72F03F392E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666BFC02-ABD6-4F92-A4F4-B610AA135E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="4100" windowWidth="25520" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bio_master_D" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="226">
   <si>
     <t>Animal</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Accipiter fasciatus</t>
   </si>
   <si>
-    <t>AccipiterÂ cooperi</t>
-  </si>
-  <si>
     <t>Acrocephalus australis</t>
   </si>
   <si>
@@ -625,6 +622,102 @@
   </si>
   <si>
     <t>Common Name</t>
+  </si>
+  <si>
+    <t>Spiny-cheeked honeyeater</t>
+  </si>
+  <si>
+    <t>Inland thornbill</t>
+  </si>
+  <si>
+    <t>Yellow-rumped thornbill</t>
+  </si>
+  <si>
+    <t>Striated thornbill</t>
+  </si>
+  <si>
+    <t>Yellow thornbill</t>
+  </si>
+  <si>
+    <t>Brown thornbill</t>
+  </si>
+  <si>
+    <t>Buff-rumped thornbill</t>
+  </si>
+  <si>
+    <t>Chestnut-rumped thornbill</t>
+  </si>
+  <si>
+    <t>Eastern spinebill</t>
+  </si>
+  <si>
+    <t>Collared sparrowhawk</t>
+  </si>
+  <si>
+    <t>Brown Goshawk</t>
+  </si>
+  <si>
+    <t>Accipiter cooperi</t>
+  </si>
+  <si>
+    <t>Cooper's hawk</t>
+  </si>
+  <si>
+    <t>Australian owlet-nightjar</t>
+  </si>
+  <si>
+    <t>Australian reed warbler</t>
+  </si>
+  <si>
+    <t>Plum-headed finch</t>
+  </si>
+  <si>
+    <t>Australian king parrot</t>
+  </si>
+  <si>
+    <t>Dusky grasswren</t>
+  </si>
+  <si>
+    <t>Pacific black duck</t>
+  </si>
+  <si>
+    <t>Eurasian skylark</t>
+  </si>
+  <si>
+    <t>Australasian darter</t>
+  </si>
+  <si>
+    <t>Magpie Goose</t>
+  </si>
+  <si>
+    <t>Red wattlebird</t>
+  </si>
+  <si>
+    <t>Regent honeyeater</t>
+  </si>
+  <si>
+    <t>Little wattlebird</t>
+  </si>
+  <si>
+    <t>Australian pipit</t>
+  </si>
+  <si>
+    <t>Sarus crane</t>
+  </si>
+  <si>
+    <t>Brolga</t>
+  </si>
+  <si>
+    <t>Southern whiteface</t>
+  </si>
+  <si>
+    <t>Red-winged parrot</t>
+  </si>
+  <si>
+    <t>Wedge-tailed eagle</t>
+  </si>
+  <si>
+    <t>Black-faced woodswallow</t>
   </si>
 </sst>
 </file>
@@ -1800,41 +1893,41 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A62:XFD83"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="45.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="29" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" style="30" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="31" customWidth="1"/>
-    <col min="10" max="10" width="27.6328125" style="32" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1"/>
-    <col min="12" max="12" width="30.90625" customWidth="1"/>
-    <col min="13" max="13" width="27.6328125" customWidth="1"/>
-    <col min="14" max="14" width="23.90625" customWidth="1"/>
-    <col min="15" max="15" width="144.7265625" customWidth="1"/>
-    <col min="16" max="16" width="60.90625" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="30" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="31" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" style="32" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="30.88671875" customWidth="1"/>
+    <col min="13" max="13" width="27.6640625" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" customWidth="1"/>
+    <col min="15" max="15" width="144.77734375" customWidth="1"/>
+    <col min="16" max="16" width="60.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="46.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
@@ -1856,16 +1949,18 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="34" t="s">
+        <v>194</v>
+      </c>
       <c r="C2" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="22"/>
@@ -1878,31 +1973,34 @@
         <v>A photo realistic images of the animal, Acanthagenys rufogularis in it's natural habitat</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O2" t="str">
         <f>_xlfn.CONCAT($P$2,A2,$Q$2)</f>
         <v>Please generate a short species bio with some interesting facts about  Acanthagenys rufogularis.</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="35" t="s">
+        <v>195</v>
+      </c>
       <c r="C3" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" s="9" t="str">
         <f t="shared" ref="L3:L61" si="0">_xlfn.CONCAT($M$2,A3,$N$2)</f>
@@ -1913,15 +2011,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza apicalis.</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="35" t="s">
+        <v>196</v>
+      </c>
       <c r="C4" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1933,15 +2034,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza chrysorrhoa.</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="35" t="s">
+        <v>197</v>
+      </c>
       <c r="C5" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1952,15 +2056,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza lineata.</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="35" t="s">
+        <v>198</v>
+      </c>
       <c r="C6" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1971,15 +2078,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza nana.</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="35" t="s">
+        <v>199</v>
+      </c>
       <c r="C7" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1990,15 +2100,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza pusilla.</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="35" t="s">
+        <v>200</v>
+      </c>
       <c r="C8" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2009,15 +2122,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza reguloides.</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="35" t="s">
+        <v>201</v>
+      </c>
       <c r="C9" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2028,15 +2144,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthiza uropygialis.</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="35" t="s">
+        <v>202</v>
+      </c>
       <c r="C10" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2047,15 +2166,18 @@
         <v>Please generate a short species bio with some interesting facts about  Acanthorhynchus tenuirostris.</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="35" t="s">
+        <v>203</v>
+      </c>
       <c r="C11" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2066,961 +2188,1024 @@
         <v>Please generate a short species bio with some interesting facts about  Accipiter cirrocephalus.</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B12" s="35" t="s">
+        <v>204</v>
+      </c>
       <c r="C12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Accipiter fasciatus in it's natural habitat</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Accipiter fasciatus.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="L12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Accipiter fasciatus in it's natural habitat</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Accipiter fasciatus.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="L13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Accipiter cooperi in it's natural habitat</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Accipiter cooperi.</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="B14" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, AccipiterÂ cooperi in it's natural habitat</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  AccipiterÂ cooperi.</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Acrocephalus australis in it's natural habitat</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Acrocephalus australis.</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="B15" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Acrocephalus australis in it's natural habitat</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Acrocephalus australis.</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="F15" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="L15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aegotheles cristatus in it's natural habitat</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aegotheles cristatus.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aegotheles cristatus in it's natural habitat</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aegotheles cristatus.</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="L16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aidemosyne modesta in it's natural habitat</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aidemosyne modesta.</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="B17" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aidemosyne modesta in it's natural habitat</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aidemosyne modesta.</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="L17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Alisterus scapularis in it's natural habitat</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Alisterus scapularis.</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="B18" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Alisterus scapularis in it's natural habitat</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Alisterus scapularis.</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="F18" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Alauda Arvensis in it's natural habitat</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Alauda Arvensis.</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="B19" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Alauda Arvensis in it's natural habitat</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Alauda Arvensis.</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="L19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Amytornis purnelli in it's natural habitat</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Amytornis purnelli.</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="B20" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D20" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="L19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Amytornis purnelli in it's natural habitat</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Amytornis purnelli.</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="L20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anas superciliosa in it's natural habitat</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anas superciliosa.</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="B21" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="L20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anas superciliosa in it's natural habitat</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anas superciliosa.</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="L21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anhinga novaehollandiae in it's natural habitat</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anhinga novaehollandiae.</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="B22" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="L21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anhinga novaehollandiae in it's natural habitat</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anhinga novaehollandiae.</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="L22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anseranas semipalmata in it's natural habitat</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anseranas semipalmata.</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="B23" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D23" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="L22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anseranas semipalmata in it's natural habitat</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anseranas semipalmata.</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="L23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anthochaera carunculata in it's natural habitat</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anthochaera carunculata.</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="B24" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D24" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="L23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anthochaera carunculata in it's natural habitat</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anthochaera carunculata.</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="L24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anthochaera chrysoptera in it's natural habitat</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anthochaera chrysoptera.</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="B25" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="L24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anthochaera chrysoptera in it's natural habitat</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anthochaera chrysoptera.</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="L25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anthochaera phrygia in it's natural habitat</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anthochaera phrygia.</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="B26" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="L25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anthochaera phrygia in it's natural habitat</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anthochaera phrygia.</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="L26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Anthus novaeseelandiae in it's natural habitat</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Anthus novaeseelandiae.</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="B27" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="L26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Anthus novaeseelandiae in it's natural habitat</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Anthus novaeseelandiae.</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="L27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Antigone antigone in it's natural habitat</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Antigone antigone.</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="B28" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="L27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Antigone antigone in it's natural habitat</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Antigone antigone.</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="L28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Antigone rubicunda in it's natural habitat</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Antigone rubicunda.</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="B29" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="L28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Antigone rubicunda in it's natural habitat</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Antigone rubicunda.</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="L29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aphelocephala leucopsis in it's natural habitat</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aphelocephala leucopsis.</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="L29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aphelocephala leucopsis in it's natural habitat</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aphelocephala leucopsis.</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="L30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, ApocritaÂ sp. in it's natural habitat</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  ApocritaÂ sp..</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="B31" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D31" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="L30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, ApocritaÂ sp. in it's natural habitat</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  ApocritaÂ sp..</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="L31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aprosmictus erythropterus in it's natural habitat</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aprosmictus erythropterus.</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="B32" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="L31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aprosmictus erythropterus in it's natural habitat</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aprosmictus erythropterus.</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="L32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aquila audax in it's natural habitat</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aquila audax.</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="B33" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D33" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="L32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aquila audax in it's natural habitat</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aquila audax.</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+      <c r="L33" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Artamus cinereus in it's natural habitat</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Artamus cinereus.</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D34" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="L33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Artamus cinereus in it's natural habitat</v>
-      </c>
-      <c r="O33" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Artamus cinereus.</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="L34" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Artamus cyanopterus in it's natural habitat</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Artamus cyanopterus.</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C35" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D35" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="L34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Artamus cyanopterus in it's natural habitat</v>
-      </c>
-      <c r="O34" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Artamus cyanopterus.</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="L35" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Artamus minor in it's natural habitat</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Artamus minor.</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D36" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L35" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Artamus minor in it's natural habitat</v>
-      </c>
-      <c r="O35" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Artamus minor.</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="L36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Artamus superciliosus in it's natural habitat</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Artamus superciliosus.</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D37" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="L36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Artamus superciliosus in it's natural habitat</v>
-      </c>
-      <c r="O36" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Artamus superciliosus.</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="L37" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Atrapsalta encaustica in it's natural habitat</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Atrapsalta encaustica.</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D38" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="L37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Atrapsalta encaustica in it's natural habitat</v>
-      </c>
-      <c r="O37" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Atrapsalta encaustica.</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="L38" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Auscala spinosa in it's natural habitat</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Auscala spinosa.</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="L38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Auscala spinosa in it's natural habitat</v>
-      </c>
-      <c r="O38" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Auscala spinosa.</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="L39" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Austrochaperina pluvialis in it's natural habitat</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Austrochaperina pluvialis.</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D40" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="L39" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Austrochaperina pluvialis in it's natural habitat</v>
-      </c>
-      <c r="O39" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Austrochaperina pluvialis.</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="L40" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Austronomus australis in it's natural habitat</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Austronomus australis.</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D41" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="L40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Austronomus australis in it's natural habitat</v>
-      </c>
-      <c r="O40" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Austronomus australis.</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
+      <c r="L41" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, AvesÂ sp. in it's natural habitat</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  AvesÂ sp..</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D42" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="L41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, AvesÂ sp. in it's natural habitat</v>
-      </c>
-      <c r="O41" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  AvesÂ sp..</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+      <c r="L42" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Aythya australis in it's natural habitat</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Aythya australis.</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D43" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="L42" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Aythya australis in it's natural habitat</v>
-      </c>
-      <c r="O42" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Aythya australis.</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
+      <c r="L43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Barnardius zonarius in it's natural habitat</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Barnardius zonarius.</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D44" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="L43" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Barnardius zonarius in it's natural habitat</v>
-      </c>
-      <c r="O43" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Barnardius zonarius.</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+      <c r="L44" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Biziura lobata in it's natural habitat</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Biziura lobata.</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D45" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="L44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Biziura lobata in it's natural habitat</v>
-      </c>
-      <c r="O44" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Biziura lobata.</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
+      <c r="L45" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Burhinus grallarius in it's natural habitat</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Burhinus grallarius.</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D46" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="L45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Burhinus grallarius in it's natural habitat</v>
-      </c>
-      <c r="O45" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Burhinus grallarius.</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="L46" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Cacatua galerita in it's natural habitat</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Cacatua galerita.</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C47" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D47" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="L46" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Cacatua galerita in it's natural habitat</v>
-      </c>
-      <c r="O46" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Cacatua galerita.</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
+      <c r="L47" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Cacatua sanguinea in it's natural habitat</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Cacatua sanguinea.</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C48" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D48" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="L47" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Cacatua sanguinea in it's natural habitat</v>
-      </c>
-      <c r="O47" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Cacatua sanguinea.</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+      <c r="L48" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Cacomantis flabelliformis in it's natural habitat</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Cacomantis flabelliformis.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C49" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D49" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="L48" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Cacomantis flabelliformis in it's natural habitat</v>
-      </c>
-      <c r="O48" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Cacomantis flabelliformis.</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="L49" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Cacomantis variolosus in it's natural habitat</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Cacomantis variolosus.</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C50" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D50" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="L49" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Cacomantis variolosus in it's natural habitat</v>
-      </c>
-      <c r="O49" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Cacomantis variolosus.</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+      <c r="L50" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, CaeliferaÂ sp. in it's natural habitat</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  CaeliferaÂ sp..</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C51" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D51" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="L50" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, CaeliferaÂ sp. in it's natural habitat</v>
-      </c>
-      <c r="O50" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  CaeliferaÂ sp..</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
+      <c r="F51" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Caligavis chrysops in it's natural habitat</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Caligavis chrysops.</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C52" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D52" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="F51" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L51" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Caligavis chrysops in it's natural habitat</v>
-      </c>
-      <c r="O51" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Caligavis chrysops.</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+      <c r="L52" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Callocephalon fimbriatum in it's natural habitat</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Callocephalon fimbriatum.</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C53" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D53" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="L52" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Callocephalon fimbriatum in it's natural habitat</v>
-      </c>
-      <c r="O52" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Callocephalon fimbriatum.</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+      <c r="L53" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Calyptorhynchus banksii in it's natural habitat</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Calyptorhynchus banksii.</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C54" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D54" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="L53" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Calyptorhynchus banksii in it's natural habitat</v>
-      </c>
-      <c r="O53" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Calyptorhynchus banksii.</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="L54" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Calyptorhynchus lathami in it's natural habitat</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Calyptorhynchus lathami.</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D55" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Calyptorhynchus lathami in it's natural habitat</v>
-      </c>
-      <c r="O54" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Calyptorhynchus lathami.</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+      <c r="L55" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Canis familiaris in it's natural habitat</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Canis familiaris.</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D56" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="L55" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Canis familiaris in it's natural habitat</v>
-      </c>
-      <c r="O55" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Canis familiaris.</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="F56" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Capra hircus in it's natural habitat</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Capra hircus.</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C57" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D57" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="F56" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L56" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Capra hircus in it's natural habitat</v>
-      </c>
-      <c r="O56" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Capra hircus.</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+      <c r="L57" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Carduelis carduelis in it's natural habitat</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Carduelis carduelis.</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C58" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D58" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="L57" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Carduelis carduelis in it's natural habitat</v>
-      </c>
-      <c r="O57" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Carduelis carduelis.</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+      <c r="L58" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Carterornis leucotis in it's natural habitat</v>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Carterornis leucotis.</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C59" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D59" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L58" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Carterornis leucotis in it's natural habitat</v>
-      </c>
-      <c r="O58" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Carterornis leucotis.</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+      <c r="L59" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Centropus phasianinus in it's natural habitat</v>
+      </c>
+      <c r="O59" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Centropus phasianinus.</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C60" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D60" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="L59" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Centropus phasianinus in it's natural habitat</v>
-      </c>
-      <c r="O59" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Centropus phasianinus.</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+      <c r="F60" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L60" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>A photo realistic images of the animal, Cervus Unicolour in it's natural habitat</v>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="1"/>
+        <v>Please generate a short species bio with some interesting facts about  Cervus Unicolour.</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C61" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D61" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="F60" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L60" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>A photo realistic images of the animal, Cervus Unicolour in it's natural habitat</v>
-      </c>
-      <c r="O60" t="str">
-        <f t="shared" si="1"/>
-        <v>Please generate a short species bio with some interesting facts about  Cervus Unicolour.</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="L61" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>